<commit_message>
added better-looking error warnings for empty cells made the parser more user-independent
</commit_message>
<xml_diff>
--- a/ToParse_Python.xlsx
+++ b/ToParse_Python.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t xml:space="preserve">Quote Number</t>
   </si>
@@ -82,7 +82,25 @@
     <t xml:space="preserve">Really Good, Give Him a chance</t>
   </si>
   <si>
+    <t xml:space="preserve">------</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JKL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seriously Man? </t>
+  </si>
+  <si>
+    <t xml:space="preserve">No-ware</t>
+  </si>
+  <si>
     <t xml:space="preserve">-----------</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MNO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is okay okay</t>
   </si>
 </sst>
 </file>
@@ -200,10 +218,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:G14"/>
+  <dimension ref="B2:G15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -243,83 +261,121 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="0" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="2" t="s">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="D8" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="D9" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>13</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>200.2</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="G10" s="0" t="n">
-        <v>200.2</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>100.1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>100.1</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C12" s="0" t="n">
-        <v>3</v>
-      </c>
+        <v>123.34</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="0" t="n">
-        <v>123.34</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
     <row r="14" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C15" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>121.12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the ----------- test case in the xlsx
Known issue: the ------------ should be in the list columns to end the parsing
</commit_message>
<xml_diff>
--- a/ToParse_Python.xlsx
+++ b/ToParse_Python.xlsx
@@ -94,7 +94,7 @@
     <t xml:space="preserve">No-ware</t>
   </si>
   <si>
-    <t xml:space="preserve">-----------</t>
+    <t xml:space="preserve">------------</t>
   </si>
   <si>
     <t xml:space="preserve">MNO</t>
@@ -111,7 +111,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -140,6 +140,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -184,7 +190,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -198,6 +204,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -221,7 +231,7 @@
   <dimension ref="B2:G15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -356,8 +366,9 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="3" t="s">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="3"/>
+      <c r="E14" s="4" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed the test case to be more descriptive
</commit_message>
<xml_diff>
--- a/ToParse_Python.xlsx
+++ b/ToParse_Python.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t xml:space="preserve">Quote Number</t>
   </si>
@@ -83,6 +83,9 @@
   </si>
   <si>
     <t xml:space="preserve">------</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Less than 10 dash. Should not stop</t>
   </si>
   <si>
     <t xml:space="preserve">JKL</t>
@@ -111,7 +114,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -140,12 +143,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -190,7 +187,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -204,10 +201,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -231,7 +224,7 @@
   <dimension ref="B2:G15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -348,19 +341,22 @@
       <c r="D12" s="0" t="s">
         <v>19</v>
       </c>
+      <c r="E12" s="0" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="n">
         <v>4</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G13" s="0" t="n">
         <v>0.01</v>
@@ -368,8 +364,8 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="3"/>
-      <c r="E14" s="4" t="s">
-        <v>23</v>
+      <c r="E14" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -377,10 +373,10 @@
         <v>5</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
V 0.1: Adds the detection of the dashes outside the scope of the list in the sheet
</commit_message>
<xml_diff>
--- a/ToParse_Python.xlsx
+++ b/ToParse_Python.xlsx
@@ -97,7 +97,7 @@
     <t xml:space="preserve">No-ware</t>
   </si>
   <si>
-    <t xml:space="preserve">------------</t>
+    <t xml:space="preserve">-------------</t>
   </si>
   <si>
     <t xml:space="preserve">MNO</t>
@@ -224,7 +224,7 @@
   <dimension ref="B2:G15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -363,10 +363,10 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="3"/>
-      <c r="E14" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="n">

</xml_diff>